<commit_message>
Corey and Max wrote failing tests for reading from a file and testing robot queue
</commit_message>
<xml_diff>
--- a/mINE.xlsx
+++ b/mINE.xlsx
@@ -389,15 +389,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T20"/>
+  <dimension ref="A1:U21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U6" sqref="U6"/>
+      <selection activeCell="Y19" sqref="Y19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -458,8 +458,11 @@
       <c r="T1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -520,8 +523,11 @@
       <c r="T2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -582,8 +588,11 @@
       <c r="T3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -644,8 +653,11 @@
       <c r="T4" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -706,8 +718,11 @@
       <c r="T5" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -768,8 +783,11 @@
       <c r="T6" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -830,8 +848,11 @@
       <c r="T7" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -892,8 +913,11 @@
       <c r="T8" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -954,8 +978,11 @@
       <c r="T9" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -1016,8 +1043,11 @@
       <c r="T10" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -1078,8 +1108,11 @@
       <c r="T11" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -1140,8 +1173,11 @@
       <c r="T12" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -1202,8 +1238,11 @@
       <c r="T13" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -1264,8 +1303,11 @@
       <c r="T14" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -1326,8 +1368,11 @@
       <c r="T15" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -1388,8 +1433,11 @@
       <c r="T16" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>0</v>
       </c>
@@ -1450,8 +1498,11 @@
       <c r="T17" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>0</v>
       </c>
@@ -1512,8 +1563,11 @@
       <c r="T18" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U18">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>0</v>
       </c>
@@ -1574,8 +1628,11 @@
       <c r="T19" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U19">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>0</v>
       </c>
@@ -1635,6 +1692,71 @@
       </c>
       <c r="T20" t="s">
         <v>2</v>
+      </c>
+      <c r="U20">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>0</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+      <c r="D21">
+        <v>3</v>
+      </c>
+      <c r="E21">
+        <v>4</v>
+      </c>
+      <c r="F21">
+        <v>5</v>
+      </c>
+      <c r="G21">
+        <v>6</v>
+      </c>
+      <c r="H21">
+        <v>7</v>
+      </c>
+      <c r="I21">
+        <v>8</v>
+      </c>
+      <c r="J21">
+        <v>9</v>
+      </c>
+      <c r="K21">
+        <v>10</v>
+      </c>
+      <c r="L21">
+        <v>11</v>
+      </c>
+      <c r="M21">
+        <v>12</v>
+      </c>
+      <c r="N21">
+        <v>13</v>
+      </c>
+      <c r="O21">
+        <v>14</v>
+      </c>
+      <c r="P21">
+        <v>15</v>
+      </c>
+      <c r="Q21">
+        <v>16</v>
+      </c>
+      <c r="R21">
+        <v>17</v>
+      </c>
+      <c r="S21">
+        <v>18</v>
+      </c>
+      <c r="T21">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Drew a more complex mine and refactored everywhere where the number of caverns was hardcoded
</commit_message>
<xml_diff>
--- a/mINE.xlsx
+++ b/mINE.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="22995" windowHeight="10035"/>
+    <workbookView xWindow="3900" yWindow="3420" windowWidth="30040" windowHeight="16140"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -43,10 +48,26 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -81,15 +102,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -392,12 +417,12 @@
   <dimension ref="A1:U21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Y19" sqref="Y19"/>
+      <selection activeCell="O1" sqref="O1:O3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="3.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="3.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -462,7 +487,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -527,7 +552,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -592,7 +617,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -657,7 +682,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -722,7 +747,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -787,7 +812,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -852,7 +877,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -917,7 +942,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -982,7 +1007,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -1047,7 +1072,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -1112,7 +1137,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -1177,7 +1202,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -1242,7 +1267,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -1307,7 +1332,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -1372,7 +1397,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -1437,7 +1462,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21">
       <c r="A17" t="s">
         <v>0</v>
       </c>
@@ -1502,7 +1527,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21">
       <c r="A18" t="s">
         <v>0</v>
       </c>
@@ -1567,7 +1592,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21">
       <c r="A19" t="s">
         <v>0</v>
       </c>
@@ -1632,7 +1657,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21">
       <c r="A20" t="s">
         <v>0</v>
       </c>
@@ -1697,7 +1722,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21">
       <c r="A21">
         <v>0</v>
       </c>
@@ -1761,6 +1786,12 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1770,9 +1801,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1782,8 +1818,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>